<commit_message>
Primeira etapa do simulador de batalha adicionado
</commit_message>
<xml_diff>
--- a/Entities/Data/MovesPokemon.xlsx
+++ b/Entities/Data/MovesPokemon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16200" windowHeight="11955"/>
+    <workbookView windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -89,9 +89,6 @@
     <t>RAZOR LEAF</t>
   </si>
   <si>
-    <t>d8</t>
-  </si>
-  <si>
     <t>FOLHA NAVALHA</t>
   </si>
   <si>
@@ -164,7 +161,7 @@
     <t>TAIL WHIP</t>
   </si>
   <si>
-    <t>W.TWODICES;B.TWODICES</t>
+    <t>W.TWODICES</t>
   </si>
   <si>
     <t>CAUDA CHICOTE</t>
@@ -207,17 +204,195 @@
   </si>
   <si>
     <t>HIDRO-BOMBA</t>
+  </si>
+  <si>
+    <t>STRING SHOT</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>TIRO DE ESTILINGUE</t>
+  </si>
+  <si>
+    <t>POISON STING</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>PICADA VENENOSA</t>
+  </si>
+  <si>
+    <t>HARDEN</t>
+  </si>
+  <si>
+    <t>ENDURECER</t>
+  </si>
+  <si>
+    <t>VENOSHOCK</t>
+  </si>
+  <si>
+    <t>ESPECIAL</t>
+  </si>
+  <si>
+    <t>VENOCHOQUE</t>
+  </si>
+  <si>
+    <t>PIN MISSILE</t>
+  </si>
+  <si>
+    <t>MÍSSIL ESPINHO</t>
+  </si>
+  <si>
+    <t>SAND ATTACK</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>ATAQUE DE AREIA</t>
+  </si>
+  <si>
+    <t>GUST</t>
+  </si>
+  <si>
+    <t>VENTANIA</t>
+  </si>
+  <si>
+    <t>QUICK ATTACK</t>
+  </si>
+  <si>
+    <t>W.FIRST</t>
+  </si>
+  <si>
+    <t>ATAQUE RÁPIDO</t>
+  </si>
+  <si>
+    <t>WHIRWIND</t>
+  </si>
+  <si>
+    <t>B.CHANGE</t>
+  </si>
+  <si>
+    <t>RAJADA DE VENTO</t>
+  </si>
+  <si>
+    <t>AIR SLASH</t>
+  </si>
+  <si>
+    <t>GOLPE DE AR</t>
+  </si>
+  <si>
+    <t>DEFOG</t>
+  </si>
+  <si>
+    <t>DESNEBLINAR</t>
+  </si>
+  <si>
+    <t>PSYBEAM</t>
+  </si>
+  <si>
+    <t>Psychic</t>
+  </si>
+  <si>
+    <t>RAIO PSÍQUICO</t>
+  </si>
+  <si>
+    <t>THUNDER SHOCK</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>B.PARALYZE</t>
+  </si>
+  <si>
+    <t>CHOQUE TROVÃO</t>
+  </si>
+  <si>
+    <t>THUNDER PUNCH</t>
+  </si>
+  <si>
+    <t>SOCO TROVÃO</t>
+  </si>
+  <si>
+    <t>ELECTRIC BALL</t>
+  </si>
+  <si>
+    <t>W.HALFLEVEL</t>
+  </si>
+  <si>
+    <t>BOLA ELÉTRICA</t>
+  </si>
+  <si>
+    <t>HYPER FANG</t>
+  </si>
+  <si>
+    <t>MEGA PRESA</t>
+  </si>
+  <si>
+    <t>SUPER FANG</t>
+  </si>
+  <si>
+    <t>B.HALFLEVEL</t>
+  </si>
+  <si>
+    <t>SUPER PRESA</t>
+  </si>
+  <si>
+    <t>MIRROR MOVE</t>
+  </si>
+  <si>
+    <t>DRILL PECK</t>
+  </si>
+  <si>
+    <t>PECK</t>
+  </si>
+  <si>
+    <t>BICADA</t>
+  </si>
+  <si>
+    <t>LEER</t>
+  </si>
+  <si>
+    <t>ENCARAR</t>
+  </si>
+  <si>
+    <t>ACID</t>
+  </si>
+  <si>
+    <t>ÁCIDO</t>
+  </si>
+  <si>
+    <t>BITE</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>MORDIDA</t>
+  </si>
+  <si>
+    <t>WRAP</t>
+  </si>
+  <si>
+    <t>W.SOMADICES</t>
+  </si>
+  <si>
+    <t>ENRROLAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -827,8 +1002,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,6 +1057,18 @@
     <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -891,8 +1079,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J19" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:J19" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J43" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:J43" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="NAME"/>
@@ -900,7 +1088,7 @@
     <tableColumn id="4" name="TYPE"/>
     <tableColumn id="5" name="DICE"/>
     <tableColumn id="6" name="EFFECT"/>
-    <tableColumn id="7" name="EFROLL"/>
+    <tableColumn id="7" name="EFROLL" dataDxfId="0"/>
     <tableColumn id="8" name="PT.NAME"/>
     <tableColumn id="9" name="SP.NAME"/>
     <tableColumn id="10" name="JP.NAME"/>
@@ -1167,10 +1355,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1179,8 +1367,8 @@
     <col min="2" max="2" width="25.0571428571429" customWidth="1"/>
     <col min="3" max="3" width="7.25714285714286" customWidth="1"/>
     <col min="5" max="5" width="6.77142857142857" customWidth="1"/>
-    <col min="6" max="6" width="13.3904761904762" customWidth="1"/>
-    <col min="7" max="7" width="9.38095238095238" customWidth="1"/>
+    <col min="6" max="6" width="14.6857142857143" customWidth="1"/>
+    <col min="7" max="7" width="9.38095238095238" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.3619047619048" customWidth="1"/>
     <col min="9" max="9" width="14.2761904761905" customWidth="1"/>
     <col min="10" max="10" width="14.6" customWidth="1"/>
@@ -1205,7 +1393,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1268,7 +1456,7 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -1288,11 +1476,11 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
         <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1300,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1309,13 +1497,13 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
         <v>23</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1323,7 +1511,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1332,10 +1520,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
         <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1343,22 +1531,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
         <v>30</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1366,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1375,10 +1563,10 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
         <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1386,22 +1574,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1409,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1417,11 +1605,11 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
-        <v>20</v>
+      <c r="E11">
+        <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1429,22 +1617,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1452,16 +1640,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
         <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1469,7 +1657,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1478,10 +1666,10 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
         <v>45</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1489,16 +1677,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
         <v>48</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1506,19 +1694,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
         <v>51</v>
-      </c>
-      <c r="H16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1526,22 +1714,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
         <v>54</v>
-      </c>
-      <c r="G17">
-        <v>6</v>
-      </c>
-      <c r="H17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1549,7 +1737,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1558,10 +1746,10 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1569,19 +1757,517 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>59</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="1">
+        <v>6</v>
+      </c>
+      <c r="H41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="1">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A43">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B43">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Sistema de Box com Profiles; Personalização de Pokémon; Status Conditions; Item cards e melhorias no combate
</commit_message>
<xml_diff>
--- a/Entities/Data/MovesPokemon.xlsx
+++ b/Entities/Data/MovesPokemon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="10110"/>
+    <workbookView windowWidth="16935" windowHeight="11865"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
   <si>
     <t>ID</t>
   </si>
@@ -242,6 +242,9 @@
     <t>PIN MISSILE</t>
   </si>
   <si>
+    <t>W.SOMADICES</t>
+  </si>
+  <si>
     <t>MÍSSIL ESPINHO</t>
   </si>
   <si>
@@ -377,10 +380,64 @@
     <t>WRAP</t>
   </si>
   <si>
-    <t>W.SOMADICES</t>
-  </si>
-  <si>
     <t>ENRROLAR</t>
+  </si>
+  <si>
+    <t>SCRATCH</t>
+  </si>
+  <si>
+    <t>ARRANHAR</t>
+  </si>
+  <si>
+    <t>HORN ATTACK</t>
+  </si>
+  <si>
+    <t>ATAQUE DE CHIFRE</t>
+  </si>
+  <si>
+    <t>HORN DRILL</t>
+  </si>
+  <si>
+    <t>B.KO</t>
+  </si>
+  <si>
+    <t>CHIFRE BROCA</t>
+  </si>
+  <si>
+    <t>THRASH</t>
+  </si>
+  <si>
+    <t>W.CONFUSION</t>
+  </si>
+  <si>
+    <t>SWIFT</t>
+  </si>
+  <si>
+    <t>W.PRECISION</t>
+  </si>
+  <si>
+    <t>ATAQUE SURPRESA</t>
+  </si>
+  <si>
+    <t>DIG</t>
+  </si>
+  <si>
+    <t>CAVAR</t>
+  </si>
+  <si>
+    <t>DOUBLE KICK</t>
+  </si>
+  <si>
+    <t>Fighting</t>
+  </si>
+  <si>
+    <t>CHUTE DUPLO</t>
+  </si>
+  <si>
+    <t>BODYSLAM</t>
+  </si>
+  <si>
+    <t>GOLPE DE CORPO</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1136,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J43" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:J43" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J51" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:J51" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="NAME"/>
@@ -1355,10 +1412,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1866,13 +1923,13 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="G24" s="1">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1880,19 +1937,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1900,7 +1957,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1909,7 +1966,7 @@
         <v>41</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1917,7 +1974,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1926,10 +1983,10 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1937,7 +1994,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1946,10 +2003,10 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1957,7 +2014,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1972,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1980,7 +2037,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1992,7 +2049,7 @@
         <v>68</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2000,13 +2057,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
         <v>53</v>
@@ -2015,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="H31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2023,22 +2080,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G32" s="1">
         <v>6</v>
       </c>
       <c r="H32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2046,19 +2103,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="G33" s="1">
+        <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2066,19 +2126,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2086,7 +2146,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2098,7 +2158,7 @@
         <v>32</v>
       </c>
       <c r="H35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2106,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2115,10 +2175,10 @@
         <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2126,7 +2186,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2143,7 +2203,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2157,7 +2217,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2166,7 +2226,7 @@
         <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2174,7 +2234,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2186,7 +2246,7 @@
         <v>44</v>
       </c>
       <c r="H40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2194,7 +2254,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2209,7 +2269,7 @@
         <v>6</v>
       </c>
       <c r="H41" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2217,13 +2277,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F42" t="s">
         <v>32</v>
@@ -2232,7 +2292,7 @@
         <v>5</v>
       </c>
       <c r="H42" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2240,7 +2300,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2252,7 +2312,7 @@
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="G43" s="1">
         <v>4</v>
@@ -2261,11 +2321,168 @@
         <v>117</v>
       </c>
     </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="1">
+        <v>5</v>
+      </c>
+      <c r="H46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
+        <v>126</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A43">
+  <conditionalFormatting sqref="A2:A51">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B43">
+  <conditionalFormatting sqref="B2:B51">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Melhorias no profile e batalha, salvamento e battlelog
</commit_message>
<xml_diff>
--- a/Entities/Data/MovesPokemon.xlsx
+++ b/Entities/Data/MovesPokemon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16935" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -438,20 +438,151 @@
   </si>
   <si>
     <t>GOLPE DE CORPO</t>
+  </si>
+  <si>
+    <t>SING</t>
+  </si>
+  <si>
+    <t>B.SLEEP</t>
+  </si>
+  <si>
+    <t>CANÇÃO</t>
+  </si>
+  <si>
+    <t>POUND</t>
+  </si>
+  <si>
+    <t>TAPA</t>
+  </si>
+  <si>
+    <t>DOUBLE SLAP</t>
+  </si>
+  <si>
+    <t>TAPA DUPLO</t>
+  </si>
+  <si>
+    <t>METRONOME</t>
+  </si>
+  <si>
+    <t>METRONOMO</t>
+  </si>
+  <si>
+    <t>FIRE SPIN</t>
+  </si>
+  <si>
+    <t>CÍRCULO DE FOGO</t>
+  </si>
+  <si>
+    <t>DISARMING VOICE</t>
+  </si>
+  <si>
+    <t>Fairy</t>
+  </si>
+  <si>
+    <t>VOZ DESARMANTE</t>
+  </si>
+  <si>
+    <t>PLAY ROUGH</t>
+  </si>
+  <si>
+    <t>BRIGAR</t>
+  </si>
+  <si>
+    <t>SUPERSONIC</t>
+  </si>
+  <si>
+    <t>SUPERSÔNICO</t>
+  </si>
+  <si>
+    <t>ANTONISH</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>ASSUSTAR</t>
+  </si>
+  <si>
+    <t>POISON FANG</t>
+  </si>
+  <si>
+    <t>PRESA VENENO</t>
+  </si>
+  <si>
+    <t>AIR CUTTER</t>
+  </si>
+  <si>
+    <t>AR CORTANTE</t>
+  </si>
+  <si>
+    <t>ABSORB</t>
+  </si>
+  <si>
+    <t>ABSORÇÃO</t>
+  </si>
+  <si>
+    <t>STUN SPORE</t>
+  </si>
+  <si>
+    <t>PÓ ATORDOANTE</t>
+  </si>
+  <si>
+    <t>PETAL DANCE</t>
+  </si>
+  <si>
+    <t>W.SLEEP</t>
+  </si>
+  <si>
+    <t>DANÇA DE PÉTALAS</t>
+  </si>
+  <si>
+    <t>SLUDGE WAVE</t>
+  </si>
+  <si>
+    <t>ONDA DE LAMA</t>
+  </si>
+  <si>
+    <t>SPORE</t>
+  </si>
+  <si>
+    <t>ESPOROS</t>
+  </si>
+  <si>
+    <t>CONFUSION</t>
+  </si>
+  <si>
+    <t>CONFUSÃO</t>
+  </si>
+  <si>
+    <t>SLEEP POWDER</t>
+  </si>
+  <si>
+    <t>PÓ DO SONO</t>
+  </si>
+  <si>
+    <t>LEECH LIFE</t>
+  </si>
+  <si>
+    <t>W.LIFE</t>
+  </si>
+  <si>
+    <t>DRENO DE VIDA</t>
+  </si>
+  <si>
+    <t>MOVIMENTO ESPELHO</t>
+  </si>
+  <si>
+    <t>BICADA FURADEIRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,353 +590,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -813,310 +607,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
-    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
-    <cellStyle name="Observação" xfId="8" builtinId="10"/>
-    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
-    <cellStyle name="Título" xfId="10" builtinId="15"/>
-    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
-    <cellStyle name="Saída" xfId="17" builtinId="21"/>
-    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
-    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
-    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Bom" xfId="22" builtinId="26"/>
-    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
-    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
-    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
-    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
-    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
-    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
-    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1136,8 +647,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J51" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:J51" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J70" totalsRowShown="0">
+  <autoFilter ref="A1:J70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="NAME"/>
@@ -1406,29 +917,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.05714285714286" customWidth="1"/>
-    <col min="2" max="2" width="25.0571428571429" customWidth="1"/>
-    <col min="3" max="3" width="7.25714285714286" customWidth="1"/>
-    <col min="5" max="5" width="6.77142857142857" customWidth="1"/>
-    <col min="6" max="6" width="14.6857142857143" customWidth="1"/>
-    <col min="7" max="7" width="9.38095238095238" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3619047619048" customWidth="1"/>
-    <col min="9" max="9" width="14.2761904761905" customWidth="1"/>
-    <col min="10" max="10" width="14.6" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1463,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1480,7 +991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1497,7 +1008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1520,7 +1031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1540,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1563,7 +1074,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1583,7 +1094,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1606,7 +1117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1626,7 +1137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1649,7 +1160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1669,7 +1180,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1692,7 +1203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1709,7 +1220,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1729,7 +1240,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1746,7 +1257,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2181,7 +1692,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2197,8 +1708,11 @@
       <c r="F37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="H37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2210,6 +1724,9 @@
       </c>
       <c r="D38" t="s">
         <v>41</v>
+      </c>
+      <c r="H38" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2378,7 +1895,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2474,19 +1991,437 @@
       <c r="F51" t="s">
         <v>93</v>
       </c>
+      <c r="G51" s="1">
+        <v>5</v>
+      </c>
       <c r="H51" t="s">
         <v>136</v>
       </c>
     </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="1">
+        <v>4</v>
+      </c>
+      <c r="H52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="1">
+        <v>4</v>
+      </c>
+      <c r="H54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>68</v>
+      </c>
+      <c r="H55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" s="1">
+        <v>4</v>
+      </c>
+      <c r="H56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>149</v>
+      </c>
+      <c r="F57" t="s">
+        <v>128</v>
+      </c>
+      <c r="H57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>149</v>
+      </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="1">
+        <v>6</v>
+      </c>
+      <c r="H58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
+        <v>53</v>
+      </c>
+      <c r="G59" s="1">
+        <v>4</v>
+      </c>
+      <c r="H59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+      <c r="F60" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="1">
+        <v>5</v>
+      </c>
+      <c r="H60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="F61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4</v>
+      </c>
+      <c r="H61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+      <c r="H62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
+        <v>93</v>
+      </c>
+      <c r="G64" s="1">
+        <v>3</v>
+      </c>
+      <c r="H64" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G65" s="1">
+        <v>5</v>
+      </c>
+      <c r="H65" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="1">
+        <v>6</v>
+      </c>
+      <c r="H66" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="s">
+        <v>138</v>
+      </c>
+      <c r="H67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>89</v>
+      </c>
+      <c r="F68" t="s">
+        <v>138</v>
+      </c>
+      <c r="G68" s="1">
+        <v>6</v>
+      </c>
+      <c r="H68" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>138</v>
+      </c>
+      <c r="G69" s="1">
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>60</v>
+      </c>
+      <c r="F70" t="s">
+        <v>178</v>
+      </c>
+      <c r="H70" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A51">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A2:A70">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B51">
+  <conditionalFormatting sqref="B2:B70">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>